<commit_message>
Finished Alt. This will be it for today
</commit_message>
<xml_diff>
--- a/Excel_Challenge_518 - Rank Students.xlsx
+++ b/Excel_Challenge_518 - Rank Students.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088A91C0-E7EC-4F7C-89DE-B1B2DAB65E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E78847-F0EC-447D-82B1-C1B38112EB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Alt!$A$1:$C$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$A$1:$C$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$A$1:$C$20</definedName>
   </definedNames>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -683,6 +685,33 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="663" row="9">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{8C508D32-F400-4323-9A26-B6D6E15B9FA0}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
@@ -922,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C21747E-DC42-4951-B201-46202E01D809}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1333,4 +1362,351 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A518FB8-45BC-4D41-93F0-3530C2CC9242}">
+  <dimension ref="A1:H43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="str" cm="1">
+        <f t="array" ref="A25:A43">_xlfn.LET(
+    _xlpm.g, B2:B20,
+    _xlpm.u, _xlfn.UNIQUE(_xlpm.g),
+    IF(
+        _xlpm.g = "F",
+        "",
+        _xlfn.XMATCH(
+            _xlpm.g,
+            _xlfn.SORTBY(
+                _xlpm.u,
+                LEFT(_xlpm.u),
+                ,
+                MID(_xlpm.u &amp; ",", 2, 1),
+                -1
+            )
+        )
+    )
+)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>